<commit_message>
Start tp3, update tp2-reporte.md, update graphics
</commit_message>
<xml_diff>
--- a/tp2-agentes-racionales/images/results.xlsx
+++ b/tp2-agentes-racionales/images/results.xlsx
@@ -2934,7 +2934,7 @@
         <v>6</v>
       </c>
       <c r="CH3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="CI3" t="n">
         <v>6</v>
@@ -2982,7 +2982,7 @@
         <v>13</v>
       </c>
       <c r="CX3" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="CY3" t="n">
         <v>26</v>
@@ -2997,7 +2997,7 @@
         <v>26</v>
       </c>
       <c r="DC3" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="DD3" t="n">
         <v>26</v>
@@ -3027,499 +3027,499 @@
         <v>51</v>
       </c>
       <c r="DM3" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="DN3" t="n">
         <v>51</v>
       </c>
       <c r="DO3" t="n">
+        <v>51</v>
+      </c>
+      <c r="DP3" t="n">
         <v>50</v>
-      </c>
-      <c r="DP3" t="n">
-        <v>51</v>
       </c>
       <c r="DQ3" t="n">
         <v>51</v>
       </c>
       <c r="DR3" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="DS3" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="DT3" t="n">
         <v>23</v>
       </c>
       <c r="DU3" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="DV3" t="n">
         <v>18</v>
       </c>
       <c r="DW3" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="DX3" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="DY3" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="DZ3" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="EA3" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="EB3" t="n">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="EC3" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="ED3" t="n">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="EE3" t="n">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="EF3" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="EG3" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="EH3" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="EI3" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="EJ3" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="EK3" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="EL3" t="n">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="EM3" t="n">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="EN3" t="n">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="EO3" t="n">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="EP3" t="n">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="EQ3" t="n">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="ER3" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="ES3" t="n">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="ET3" t="n">
         <v>75</v>
       </c>
       <c r="EU3" t="n">
+        <v>73</v>
+      </c>
+      <c r="EV3" t="n">
+        <v>138</v>
+      </c>
+      <c r="EW3" t="n">
+        <v>141</v>
+      </c>
+      <c r="EX3" t="n">
+        <v>149</v>
+      </c>
+      <c r="EY3" t="n">
+        <v>140</v>
+      </c>
+      <c r="EZ3" t="n">
+        <v>120</v>
+      </c>
+      <c r="FA3" t="n">
+        <v>152</v>
+      </c>
+      <c r="FB3" t="n">
+        <v>148</v>
+      </c>
+      <c r="FC3" t="n">
+        <v>170</v>
+      </c>
+      <c r="FD3" t="n">
+        <v>133</v>
+      </c>
+      <c r="FE3" t="n">
+        <v>162</v>
+      </c>
+      <c r="FF3" t="n">
+        <v>23</v>
+      </c>
+      <c r="FG3" t="n">
+        <v>29</v>
+      </c>
+      <c r="FH3" t="n">
+        <v>14</v>
+      </c>
+      <c r="FI3" t="n">
+        <v>20</v>
+      </c>
+      <c r="FJ3" t="n">
+        <v>29</v>
+      </c>
+      <c r="FK3" t="n">
+        <v>24</v>
+      </c>
+      <c r="FL3" t="n">
+        <v>16</v>
+      </c>
+      <c r="FM3" t="n">
+        <v>25</v>
+      </c>
+      <c r="FN3" t="n">
+        <v>23</v>
+      </c>
+      <c r="FO3" t="n">
+        <v>9</v>
+      </c>
+      <c r="FP3" t="n">
+        <v>47</v>
+      </c>
+      <c r="FQ3" t="n">
+        <v>55</v>
+      </c>
+      <c r="FR3" t="n">
+        <v>49</v>
+      </c>
+      <c r="FS3" t="n">
+        <v>65</v>
+      </c>
+      <c r="FT3" t="n">
+        <v>45</v>
+      </c>
+      <c r="FU3" t="n">
+        <v>44</v>
+      </c>
+      <c r="FV3" t="n">
+        <v>53</v>
+      </c>
+      <c r="FW3" t="n">
+        <v>46</v>
+      </c>
+      <c r="FX3" t="n">
+        <v>49</v>
+      </c>
+      <c r="FY3" t="n">
+        <v>71</v>
+      </c>
+      <c r="FZ3" t="n">
+        <v>105</v>
+      </c>
+      <c r="GA3" t="n">
+        <v>124</v>
+      </c>
+      <c r="GB3" t="n">
+        <v>114</v>
+      </c>
+      <c r="GC3" t="n">
+        <v>125</v>
+      </c>
+      <c r="GD3" t="n">
+        <v>121</v>
+      </c>
+      <c r="GE3" t="n">
+        <v>97</v>
+      </c>
+      <c r="GF3" t="n">
+        <v>86</v>
+      </c>
+      <c r="GG3" t="n">
+        <v>139</v>
+      </c>
+      <c r="GH3" t="n">
+        <v>125</v>
+      </c>
+      <c r="GI3" t="n">
+        <v>106</v>
+      </c>
+      <c r="GJ3" t="n">
+        <v>207</v>
+      </c>
+      <c r="GK3" t="n">
+        <v>146</v>
+      </c>
+      <c r="GL3" t="n">
+        <v>163</v>
+      </c>
+      <c r="GM3" t="n">
+        <v>135</v>
+      </c>
+      <c r="GN3" t="n">
+        <v>203</v>
+      </c>
+      <c r="GO3" t="n">
+        <v>212</v>
+      </c>
+      <c r="GP3" t="n">
+        <v>179</v>
+      </c>
+      <c r="GQ3" t="n">
+        <v>228</v>
+      </c>
+      <c r="GR3" t="n">
+        <v>193</v>
+      </c>
+      <c r="GS3" t="n">
+        <v>123</v>
+      </c>
+      <c r="GT3" t="n">
+        <v>26</v>
+      </c>
+      <c r="GU3" t="n">
+        <v>57</v>
+      </c>
+      <c r="GV3" t="n">
+        <v>28</v>
+      </c>
+      <c r="GW3" t="n">
+        <v>33</v>
+      </c>
+      <c r="GX3" t="n">
+        <v>51</v>
+      </c>
+      <c r="GY3" t="n">
+        <v>35</v>
+      </c>
+      <c r="GZ3" t="n">
+        <v>32</v>
+      </c>
+      <c r="HA3" t="n">
+        <v>31</v>
+      </c>
+      <c r="HB3" t="n">
+        <v>35</v>
+      </c>
+      <c r="HC3" t="n">
+        <v>31</v>
+      </c>
+      <c r="HD3" t="n">
+        <v>71</v>
+      </c>
+      <c r="HE3" t="n">
+        <v>67</v>
+      </c>
+      <c r="HF3" t="n">
+        <v>52</v>
+      </c>
+      <c r="HG3" t="n">
+        <v>82</v>
+      </c>
+      <c r="HH3" t="n">
+        <v>50</v>
+      </c>
+      <c r="HI3" t="n">
         <v>69</v>
       </c>
-      <c r="EV3" t="n">
-        <v>134</v>
-      </c>
-      <c r="EW3" t="n">
-        <v>154</v>
-      </c>
-      <c r="EX3" t="n">
-        <v>143</v>
-      </c>
-      <c r="EY3" t="n">
-        <v>146</v>
-      </c>
-      <c r="EZ3" t="n">
-        <v>142</v>
-      </c>
-      <c r="FA3" t="n">
-        <v>155</v>
-      </c>
-      <c r="FB3" t="n">
-        <v>158</v>
-      </c>
-      <c r="FC3" t="n">
-        <v>112</v>
-      </c>
-      <c r="FD3" t="n">
-        <v>127</v>
-      </c>
-      <c r="FE3" t="n">
-        <v>138</v>
-      </c>
-      <c r="FF3" t="n">
-        <v>26</v>
-      </c>
-      <c r="FG3" t="n">
-        <v>27</v>
-      </c>
-      <c r="FH3" t="n">
-        <v>21</v>
-      </c>
-      <c r="FI3" t="n">
-        <v>31</v>
-      </c>
-      <c r="FJ3" t="n">
-        <v>44</v>
-      </c>
-      <c r="FK3" t="n">
-        <v>20</v>
-      </c>
-      <c r="FL3" t="n">
-        <v>31</v>
-      </c>
-      <c r="FM3" t="n">
-        <v>36</v>
-      </c>
-      <c r="FN3" t="n">
-        <v>33</v>
-      </c>
-      <c r="FO3" t="n">
-        <v>23</v>
-      </c>
-      <c r="FP3" t="n">
-        <v>53</v>
-      </c>
-      <c r="FQ3" t="n">
+      <c r="HJ3" t="n">
+        <v>72</v>
+      </c>
+      <c r="HK3" t="n">
+        <v>55</v>
+      </c>
+      <c r="HL3" t="n">
+        <v>71</v>
+      </c>
+      <c r="HM3" t="n">
         <v>58</v>
       </c>
-      <c r="FR3" t="n">
-        <v>68</v>
-      </c>
-      <c r="FS3" t="n">
-        <v>58</v>
-      </c>
-      <c r="FT3" t="n">
-        <v>46</v>
-      </c>
-      <c r="FU3" t="n">
-        <v>65</v>
-      </c>
-      <c r="FV3" t="n">
-        <v>58</v>
-      </c>
-      <c r="FW3" t="n">
-        <v>60</v>
-      </c>
-      <c r="FX3" t="n">
-        <v>44</v>
-      </c>
-      <c r="FY3" t="n">
-        <v>81</v>
-      </c>
-      <c r="FZ3" t="n">
-        <v>59</v>
-      </c>
-      <c r="GA3" t="n">
-        <v>83</v>
-      </c>
-      <c r="GB3" t="n">
-        <v>123</v>
-      </c>
-      <c r="GC3" t="n">
-        <v>47</v>
-      </c>
-      <c r="GD3" t="n">
+      <c r="HN3" t="n">
+        <v>94</v>
+      </c>
+      <c r="HO3" t="n">
+        <v>102</v>
+      </c>
+      <c r="HP3" t="n">
         <v>106</v>
       </c>
-      <c r="GE3" t="n">
-        <v>83</v>
-      </c>
-      <c r="GF3" t="n">
-        <v>127</v>
-      </c>
-      <c r="GG3" t="n">
-        <v>53</v>
-      </c>
-      <c r="GH3" t="n">
-        <v>105</v>
-      </c>
-      <c r="GI3" t="n">
-        <v>90</v>
-      </c>
-      <c r="GJ3" t="n">
-        <v>142</v>
-      </c>
-      <c r="GK3" t="n">
-        <v>160</v>
-      </c>
-      <c r="GL3" t="n">
-        <v>203</v>
-      </c>
-      <c r="GM3" t="n">
-        <v>140</v>
-      </c>
-      <c r="GN3" t="n">
-        <v>205</v>
-      </c>
-      <c r="GO3" t="n">
-        <v>228</v>
-      </c>
-      <c r="GP3" t="n">
-        <v>192</v>
-      </c>
-      <c r="GQ3" t="n">
-        <v>154</v>
-      </c>
-      <c r="GR3" t="n">
-        <v>167</v>
-      </c>
-      <c r="GS3" t="n">
-        <v>217</v>
-      </c>
-      <c r="GT3" t="n">
-        <v>24</v>
-      </c>
-      <c r="GU3" t="n">
-        <v>16</v>
-      </c>
-      <c r="GV3" t="n">
-        <v>23</v>
-      </c>
-      <c r="GW3" t="n">
-        <v>26</v>
-      </c>
-      <c r="GX3" t="n">
-        <v>30</v>
-      </c>
-      <c r="GY3" t="n">
-        <v>36</v>
-      </c>
-      <c r="GZ3" t="n">
-        <v>29</v>
-      </c>
-      <c r="HA3" t="n">
-        <v>24</v>
-      </c>
-      <c r="HB3" t="n">
-        <v>22</v>
-      </c>
-      <c r="HC3" t="n">
-        <v>32</v>
-      </c>
-      <c r="HD3" t="n">
-        <v>78</v>
-      </c>
-      <c r="HE3" t="n">
-        <v>70</v>
-      </c>
-      <c r="HF3" t="n">
-        <v>59</v>
-      </c>
-      <c r="HG3" t="n">
-        <v>52</v>
-      </c>
-      <c r="HH3" t="n">
-        <v>56</v>
-      </c>
-      <c r="HI3" t="n">
-        <v>72</v>
-      </c>
-      <c r="HJ3" t="n">
-        <v>54</v>
-      </c>
-      <c r="HK3" t="n">
-        <v>47</v>
-      </c>
-      <c r="HL3" t="n">
-        <v>56</v>
-      </c>
-      <c r="HM3" t="n">
-        <v>65</v>
-      </c>
-      <c r="HN3" t="n">
-        <v>130</v>
-      </c>
-      <c r="HO3" t="n">
+      <c r="HQ3" t="n">
+        <v>116</v>
+      </c>
+      <c r="HR3" t="n">
+        <v>96</v>
+      </c>
+      <c r="HS3" t="n">
         <v>118</v>
-      </c>
-      <c r="HP3" t="n">
-        <v>129</v>
-      </c>
-      <c r="HQ3" t="n">
-        <v>87</v>
-      </c>
-      <c r="HR3" t="n">
-        <v>109</v>
-      </c>
-      <c r="HS3" t="n">
-        <v>139</v>
       </c>
       <c r="HT3" t="n">
         <v>116</v>
       </c>
       <c r="HU3" t="n">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="HV3" t="n">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="HW3" t="n">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="HX3" t="n">
-        <v>199</v>
+        <v>255</v>
       </c>
       <c r="HY3" t="n">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="HZ3" t="n">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="IA3" t="n">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="IB3" t="n">
-        <v>187</v>
+        <v>236</v>
       </c>
       <c r="IC3" t="n">
+        <v>239</v>
+      </c>
+      <c r="ID3" t="n">
         <v>229</v>
       </c>
-      <c r="ID3" t="n">
-        <v>218</v>
-      </c>
       <c r="IE3" t="n">
-        <v>259</v>
+        <v>213</v>
       </c>
       <c r="IF3" t="n">
-        <v>248</v>
+        <v>184</v>
       </c>
       <c r="IG3" t="n">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="IH3" t="n">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="II3" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="IJ3" t="n">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="IK3" t="n">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="IL3" t="n">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="IM3" t="n">
         <v>38</v>
       </c>
       <c r="IN3" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="IO3" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="IP3" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="IQ3" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="IR3" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="IS3" t="n">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="IT3" t="n">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="IU3" t="n">
+        <v>67</v>
+      </c>
+      <c r="IV3" t="n">
+        <v>51</v>
+      </c>
+      <c r="IW3" t="n">
+        <v>62</v>
+      </c>
+      <c r="IX3" t="n">
         <v>69</v>
       </c>
-      <c r="IV3" t="n">
-        <v>78</v>
-      </c>
-      <c r="IW3" t="n">
-        <v>66</v>
-      </c>
-      <c r="IX3" t="n">
-        <v>47</v>
-      </c>
       <c r="IY3" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="IZ3" t="n">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="JA3" t="n">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="JB3" t="n">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="JC3" t="n">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="JD3" t="n">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="JE3" t="n">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="JF3" t="n">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="JG3" t="n">
-        <v>146</v>
+        <v>87</v>
       </c>
       <c r="JH3" t="n">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="JI3" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="JJ3" t="n">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="JK3" t="n">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="JL3" t="n">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="JM3" t="n">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="JN3" t="n">
+        <v>238</v>
+      </c>
+      <c r="JO3" t="n">
+        <v>264</v>
+      </c>
+      <c r="JP3" t="n">
+        <v>217</v>
+      </c>
+      <c r="JQ3" t="n">
+        <v>218</v>
+      </c>
+      <c r="JR3" t="n">
+        <v>248</v>
+      </c>
+      <c r="JS3" t="n">
         <v>246</v>
       </c>
-      <c r="JO3" t="n">
-        <v>247</v>
-      </c>
-      <c r="JP3" t="n">
-        <v>188</v>
-      </c>
-      <c r="JQ3" t="n">
-        <v>258</v>
-      </c>
-      <c r="JR3" t="n">
-        <v>219</v>
-      </c>
-      <c r="JS3" t="n">
-        <v>245</v>
-      </c>
       <c r="JT3" t="n">
-        <v>153</v>
+        <v>237</v>
       </c>
       <c r="JU3" t="n">
-        <v>253</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4">
@@ -3559,334 +3559,334 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
         <v>4</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
       <c r="O4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
       <c r="Q4" t="n">
+        <v>8</v>
+      </c>
+      <c r="R4" t="n">
+        <v>5</v>
+      </c>
+      <c r="S4" t="n">
         <v>0</v>
       </c>
-      <c r="R4" t="n">
-        <v>3</v>
-      </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" t="n">
+        <v>9</v>
+      </c>
+      <c r="W4" t="n">
+        <v>5</v>
+      </c>
+      <c r="X4" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>19</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AM4" t="n">
         <v>6</v>
       </c>
-      <c r="T4" t="n">
-        <v>6</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" t="n">
+      <c r="AN4" t="n">
         <v>12</v>
       </c>
-      <c r="W4" t="n">
+      <c r="AO4" t="n">
         <v>4</v>
       </c>
-      <c r="X4" t="n">
+      <c r="AP4" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>65</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>66</v>
+      </c>
+      <c r="AS4" t="n">
         <v>25</v>
       </c>
-      <c r="Y4" t="n">
-        <v>6</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>7</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>6</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>9</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>17</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>7</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>7</v>
-      </c>
-      <c r="AH4" t="n">
+      <c r="AT4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>38</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>108</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>43</v>
+      </c>
+      <c r="AX4" t="n">
         <v>15</v>
       </c>
-      <c r="AI4" t="n">
-        <v>8</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>9</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>6</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>23</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>7</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>6</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>9</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>40</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>62</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>65</v>
-      </c>
-      <c r="AS4" t="n">
+      <c r="AY4" t="n">
+        <v>82</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>22</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>24</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>36</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>75</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>138</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>49</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>61</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>73</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>52</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>34</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>69</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>280</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>33</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>119</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>138</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>58</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>98</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>87</v>
+      </c>
+      <c r="BR4" t="n">
+        <v>87</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>86</v>
+      </c>
+      <c r="BT4" t="n">
+        <v>178</v>
+      </c>
+      <c r="BU4" t="n">
+        <v>197</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>197</v>
+      </c>
+      <c r="BW4" t="n">
+        <v>89</v>
+      </c>
+      <c r="BX4" t="n">
+        <v>80</v>
+      </c>
+      <c r="BY4" t="n">
         <v>63</v>
       </c>
-      <c r="AT4" t="n">
-        <v>25</v>
-      </c>
-      <c r="AU4" t="n">
-        <v>9</v>
-      </c>
-      <c r="AV4" t="n">
-        <v>62</v>
-      </c>
-      <c r="AW4" t="n">
-        <v>21</v>
-      </c>
-      <c r="AX4" t="n">
-        <v>24</v>
-      </c>
-      <c r="AY4" t="n">
-        <v>11</v>
-      </c>
-      <c r="AZ4" t="n">
-        <v>50</v>
-      </c>
-      <c r="BA4" t="n">
-        <v>61</v>
-      </c>
-      <c r="BB4" t="n">
-        <v>10</v>
-      </c>
-      <c r="BC4" t="n">
-        <v>58</v>
-      </c>
-      <c r="BD4" t="n">
-        <v>65</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>23</v>
-      </c>
-      <c r="BF4" t="n">
-        <v>33</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>42</v>
-      </c>
-      <c r="BH4" t="n">
-        <v>36</v>
-      </c>
-      <c r="BI4" t="n">
-        <v>87</v>
-      </c>
-      <c r="BJ4" t="n">
-        <v>66</v>
-      </c>
-      <c r="BK4" t="n">
-        <v>85</v>
-      </c>
-      <c r="BL4" t="n">
-        <v>38</v>
-      </c>
-      <c r="BM4" t="n">
-        <v>81</v>
-      </c>
-      <c r="BN4" t="n">
-        <v>152</v>
-      </c>
-      <c r="BO4" t="n">
-        <v>56</v>
-      </c>
-      <c r="BP4" t="n">
-        <v>82</v>
-      </c>
-      <c r="BQ4" t="n">
-        <v>158</v>
-      </c>
-      <c r="BR4" t="n">
+      <c r="BZ4" t="n">
         <v>104</v>
       </c>
-      <c r="BS4" t="n">
-        <v>83</v>
-      </c>
-      <c r="BT4" t="n">
-        <v>62</v>
-      </c>
-      <c r="BU4" t="n">
-        <v>76</v>
-      </c>
-      <c r="BV4" t="n">
-        <v>57</v>
-      </c>
-      <c r="BW4" t="n">
-        <v>63</v>
-      </c>
-      <c r="BX4" t="n">
-        <v>165</v>
-      </c>
-      <c r="BY4" t="n">
-        <v>71</v>
-      </c>
-      <c r="BZ4" t="n">
-        <v>155</v>
-      </c>
       <c r="CA4" t="n">
-        <v>87</v>
+        <v>173</v>
       </c>
       <c r="CB4" t="n">
-        <v>118</v>
+        <v>231</v>
       </c>
       <c r="CC4" t="n">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="CD4" t="n">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="CE4" t="n">
-        <v>243</v>
+        <v>962</v>
       </c>
       <c r="CF4" t="n">
-        <v>728</v>
+        <v>314</v>
       </c>
       <c r="CG4" t="n">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="CH4" t="n">
-        <v>328</v>
+        <v>1000</v>
       </c>
       <c r="CI4" t="n">
-        <v>259</v>
+        <v>639</v>
       </c>
       <c r="CJ4" t="n">
-        <v>360</v>
+        <v>319</v>
       </c>
       <c r="CK4" t="n">
-        <v>796</v>
+        <v>536</v>
       </c>
       <c r="CL4" t="n">
-        <v>340</v>
+        <v>454</v>
       </c>
       <c r="CM4" t="n">
-        <v>394</v>
+        <v>519</v>
       </c>
       <c r="CN4" t="n">
-        <v>666</v>
+        <v>736</v>
       </c>
       <c r="CO4" t="n">
-        <v>607</v>
+        <v>342</v>
       </c>
       <c r="CP4" t="n">
-        <v>544</v>
+        <v>313</v>
       </c>
       <c r="CQ4" t="n">
+        <v>406</v>
+      </c>
+      <c r="CR4" t="n">
+        <v>765</v>
+      </c>
+      <c r="CS4" t="n">
+        <v>985</v>
+      </c>
+      <c r="CT4" t="n">
+        <v>774</v>
+      </c>
+      <c r="CU4" t="n">
+        <v>391</v>
+      </c>
+      <c r="CV4" t="n">
+        <v>462</v>
+      </c>
+      <c r="CW4" t="n">
+        <v>390</v>
+      </c>
+      <c r="CX4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="CY4" t="n">
+        <v>717</v>
+      </c>
+      <c r="CZ4" t="n">
+        <v>748</v>
+      </c>
+      <c r="DA4" t="n">
+        <v>888</v>
+      </c>
+      <c r="DB4" t="n">
+        <v>542</v>
+      </c>
+      <c r="DC4" t="n">
+        <v>303</v>
+      </c>
+      <c r="DD4" t="n">
+        <v>710</v>
+      </c>
+      <c r="DE4" t="n">
+        <v>373</v>
+      </c>
+      <c r="DF4" t="n">
+        <v>806</v>
+      </c>
+      <c r="DG4" t="n">
+        <v>258</v>
+      </c>
+      <c r="DH4" t="n">
+        <v>783</v>
+      </c>
+      <c r="DI4" t="n">
+        <v>842</v>
+      </c>
+      <c r="DJ4" t="n">
+        <v>676</v>
+      </c>
+      <c r="DK4" t="n">
+        <v>753</v>
+      </c>
+      <c r="DL4" t="n">
         <v>598</v>
       </c>
-      <c r="CR4" t="n">
-        <v>318</v>
-      </c>
-      <c r="CS4" t="n">
-        <v>484</v>
-      </c>
-      <c r="CT4" t="n">
-        <v>901</v>
-      </c>
-      <c r="CU4" t="n">
-        <v>248</v>
-      </c>
-      <c r="CV4" t="n">
-        <v>376</v>
-      </c>
-      <c r="CW4" t="n">
-        <v>608</v>
-      </c>
-      <c r="CX4" t="n">
-        <v>259</v>
-      </c>
-      <c r="CY4" t="n">
-        <v>437</v>
-      </c>
-      <c r="CZ4" t="n">
-        <v>907</v>
-      </c>
-      <c r="DA4" t="n">
-        <v>850</v>
-      </c>
-      <c r="DB4" t="n">
-        <v>527</v>
-      </c>
-      <c r="DC4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="DD4" t="n">
-        <v>504</v>
-      </c>
-      <c r="DE4" t="n">
-        <v>916</v>
-      </c>
-      <c r="DF4" t="n">
-        <v>505</v>
-      </c>
-      <c r="DG4" t="n">
-        <v>639</v>
-      </c>
-      <c r="DH4" t="n">
-        <v>512</v>
-      </c>
-      <c r="DI4" t="n">
-        <v>564</v>
-      </c>
-      <c r="DJ4" t="n">
-        <v>725</v>
-      </c>
-      <c r="DK4" t="n">
-        <v>939</v>
-      </c>
-      <c r="DL4" t="n">
-        <v>629</v>
-      </c>
       <c r="DM4" t="n">
-        <v>758</v>
+        <v>1000</v>
       </c>
       <c r="DN4" t="n">
-        <v>989</v>
+        <v>613</v>
       </c>
       <c r="DO4" t="n">
-        <v>1000</v>
+        <v>619</v>
       </c>
       <c r="DP4" t="n">
-        <v>805</v>
+        <v>1000</v>
       </c>
       <c r="DQ4" t="n">
-        <v>882</v>
+        <v>870</v>
       </c>
       <c r="DR4" t="n">
         <v>1000</v>
@@ -4556,7 +4556,7 @@
         <v>3</v>
       </c>
       <c r="BJ5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BK5" t="n">
         <v>6</v>
@@ -4616,25 +4616,25 @@
         <v>13</v>
       </c>
       <c r="CD5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="CE5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="CF5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="CG5" t="n">
         <v>6</v>
       </c>
       <c r="CH5" t="n">
+        <v>6</v>
+      </c>
+      <c r="CI5" t="n">
+        <v>3</v>
+      </c>
+      <c r="CJ5" t="n">
         <v>4</v>
-      </c>
-      <c r="CI5" t="n">
-        <v>4</v>
-      </c>
-      <c r="CJ5" t="n">
-        <v>3</v>
       </c>
       <c r="CK5" t="n">
         <v>6</v>
@@ -4643,343 +4643,343 @@
         <v>5</v>
       </c>
       <c r="CM5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="CN5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="CO5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="CP5" t="n">
+        <v>12</v>
+      </c>
+      <c r="CQ5" t="n">
+        <v>9</v>
+      </c>
+      <c r="CR5" t="n">
+        <v>8</v>
+      </c>
+      <c r="CS5" t="n">
         <v>10</v>
       </c>
-      <c r="CQ5" t="n">
+      <c r="CT5" t="n">
+        <v>9</v>
+      </c>
+      <c r="CU5" t="n">
+        <v>9</v>
+      </c>
+      <c r="CV5" t="n">
+        <v>10</v>
+      </c>
+      <c r="CW5" t="n">
         <v>13</v>
       </c>
-      <c r="CR5" t="n">
-        <v>11</v>
-      </c>
-      <c r="CS5" t="n">
-        <v>13</v>
-      </c>
-      <c r="CT5" t="n">
-        <v>10</v>
-      </c>
-      <c r="CU5" t="n">
-        <v>8</v>
-      </c>
-      <c r="CV5" t="n">
-        <v>9</v>
-      </c>
-      <c r="CW5" t="n">
-        <v>12</v>
-      </c>
       <c r="CX5" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="CY5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="CZ5" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="DA5" t="n">
+        <v>22</v>
+      </c>
+      <c r="DB5" t="n">
         <v>19</v>
-      </c>
-      <c r="DB5" t="n">
-        <v>18</v>
       </c>
       <c r="DC5" t="n">
         <v>21</v>
       </c>
       <c r="DD5" t="n">
+        <v>21</v>
+      </c>
+      <c r="DE5" t="n">
+        <v>20</v>
+      </c>
+      <c r="DF5" t="n">
         <v>19</v>
       </c>
-      <c r="DE5" t="n">
-        <v>21</v>
-      </c>
-      <c r="DF5" t="n">
-        <v>18</v>
-      </c>
       <c r="DG5" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="DH5" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="DI5" t="n">
+        <v>47</v>
+      </c>
+      <c r="DJ5" t="n">
+        <v>34</v>
+      </c>
+      <c r="DK5" t="n">
         <v>42</v>
       </c>
-      <c r="DJ5" t="n">
-        <v>45</v>
-      </c>
-      <c r="DK5" t="n">
+      <c r="DL5" t="n">
         <v>41</v>
       </c>
-      <c r="DL5" t="n">
-        <v>46</v>
-      </c>
       <c r="DM5" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="DN5" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="DO5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="DP5" t="n">
         <v>41</v>
       </c>
       <c r="DQ5" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="DR5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="DS5" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="DT5" t="n">
         <v>7</v>
       </c>
       <c r="DU5" t="n">
+        <v>8</v>
+      </c>
+      <c r="DV5" t="n">
+        <v>5</v>
+      </c>
+      <c r="DW5" t="n">
         <v>9</v>
       </c>
-      <c r="DV5" t="n">
+      <c r="DX5" t="n">
+        <v>7</v>
+      </c>
+      <c r="DY5" t="n">
+        <v>8</v>
+      </c>
+      <c r="DZ5" t="n">
         <v>9</v>
-      </c>
-      <c r="DW5" t="n">
-        <v>6</v>
-      </c>
-      <c r="DX5" t="n">
-        <v>6</v>
-      </c>
-      <c r="DY5" t="n">
-        <v>7</v>
-      </c>
-      <c r="DZ5" t="n">
-        <v>4</v>
       </c>
       <c r="EA5" t="n">
         <v>9</v>
       </c>
       <c r="EB5" t="n">
+        <v>13</v>
+      </c>
+      <c r="EC5" t="n">
         <v>17</v>
       </c>
-      <c r="EC5" t="n">
+      <c r="ED5" t="n">
+        <v>14</v>
+      </c>
+      <c r="EE5" t="n">
+        <v>15</v>
+      </c>
+      <c r="EF5" t="n">
+        <v>23</v>
+      </c>
+      <c r="EG5" t="n">
+        <v>20</v>
+      </c>
+      <c r="EH5" t="n">
+        <v>22</v>
+      </c>
+      <c r="EI5" t="n">
+        <v>16</v>
+      </c>
+      <c r="EJ5" t="n">
         <v>19</v>
       </c>
-      <c r="ED5" t="n">
+      <c r="EK5" t="n">
         <v>17</v>
       </c>
-      <c r="EE5" t="n">
-        <v>14</v>
-      </c>
-      <c r="EF5" t="n">
-        <v>18</v>
-      </c>
-      <c r="EG5" t="n">
-        <v>17</v>
-      </c>
-      <c r="EH5" t="n">
-        <v>17</v>
-      </c>
-      <c r="EI5" t="n">
-        <v>19</v>
-      </c>
-      <c r="EJ5" t="n">
-        <v>15</v>
-      </c>
-      <c r="EK5" t="n">
-        <v>18</v>
-      </c>
       <c r="EL5" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="EM5" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="EN5" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="EO5" t="n">
         <v>37</v>
       </c>
       <c r="EP5" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="EQ5" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="ER5" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="ES5" t="n">
         <v>34</v>
       </c>
       <c r="ET5" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="EU5" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="EV5" t="n">
         <v>61</v>
       </c>
       <c r="EW5" t="n">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="EX5" t="n">
+        <v>67</v>
+      </c>
+      <c r="EY5" t="n">
+        <v>68</v>
+      </c>
+      <c r="EZ5" t="n">
         <v>70</v>
       </c>
-      <c r="EY5" t="n">
-        <v>66</v>
-      </c>
-      <c r="EZ5" t="n">
-        <v>64</v>
-      </c>
       <c r="FA5" t="n">
+        <v>63</v>
+      </c>
+      <c r="FB5" t="n">
+        <v>72</v>
+      </c>
+      <c r="FC5" t="n">
+        <v>68</v>
+      </c>
+      <c r="FD5" t="n">
         <v>76</v>
       </c>
-      <c r="FB5" t="n">
-        <v>61</v>
-      </c>
-      <c r="FC5" t="n">
-        <v>67</v>
-      </c>
-      <c r="FD5" t="n">
-        <v>69</v>
-      </c>
       <c r="FE5" t="n">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="FF5" t="n">
         <v>8</v>
       </c>
       <c r="FG5" t="n">
+        <v>8</v>
+      </c>
+      <c r="FH5" t="n">
+        <v>7</v>
+      </c>
+      <c r="FI5" t="n">
+        <v>6</v>
+      </c>
+      <c r="FJ5" t="n">
+        <v>11</v>
+      </c>
+      <c r="FK5" t="n">
+        <v>6</v>
+      </c>
+      <c r="FL5" t="n">
+        <v>6</v>
+      </c>
+      <c r="FM5" t="n">
+        <v>9</v>
+      </c>
+      <c r="FN5" t="n">
+        <v>6</v>
+      </c>
+      <c r="FO5" t="n">
         <v>10</v>
       </c>
-      <c r="FH5" t="n">
-        <v>6</v>
-      </c>
-      <c r="FI5" t="n">
-        <v>12</v>
-      </c>
-      <c r="FJ5" t="n">
-        <v>8</v>
-      </c>
-      <c r="FK5" t="n">
-        <v>13</v>
-      </c>
-      <c r="FL5" t="n">
-        <v>9</v>
-      </c>
-      <c r="FM5" t="n">
-        <v>15</v>
-      </c>
-      <c r="FN5" t="n">
-        <v>8</v>
-      </c>
-      <c r="FO5" t="n">
-        <v>13</v>
-      </c>
       <c r="FP5" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="FQ5" t="n">
         <v>17</v>
       </c>
       <c r="FR5" t="n">
+        <v>11</v>
+      </c>
+      <c r="FS5" t="n">
+        <v>17</v>
+      </c>
+      <c r="FT5" t="n">
+        <v>17</v>
+      </c>
+      <c r="FU5" t="n">
+        <v>13</v>
+      </c>
+      <c r="FV5" t="n">
         <v>18</v>
       </c>
-      <c r="FS5" t="n">
-        <v>27</v>
-      </c>
-      <c r="FT5" t="n">
-        <v>15</v>
-      </c>
-      <c r="FU5" t="n">
-        <v>19</v>
-      </c>
-      <c r="FV5" t="n">
-        <v>16</v>
-      </c>
       <c r="FW5" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="FX5" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="FY5" t="n">
         <v>11</v>
       </c>
       <c r="FZ5" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="GA5" t="n">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="GB5" t="n">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="GC5" t="n">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="GD5" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="GE5" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="GF5" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="GG5" t="n">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="GH5" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="GI5" t="n">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="GJ5" t="n">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="GK5" t="n">
+        <v>55</v>
+      </c>
+      <c r="GL5" t="n">
+        <v>72</v>
+      </c>
+      <c r="GM5" t="n">
         <v>84</v>
       </c>
-      <c r="GL5" t="n">
-        <v>52</v>
-      </c>
-      <c r="GM5" t="n">
-        <v>76</v>
-      </c>
       <c r="GN5" t="n">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="GO5" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="GP5" t="n">
+        <v>80</v>
+      </c>
+      <c r="GQ5" t="n">
         <v>81</v>
       </c>
-      <c r="GQ5" t="n">
-        <v>83</v>
-      </c>
       <c r="GR5" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="GS5" t="n">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="GT5" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="GU5" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="GV5" t="n">
         <v>10</v>
@@ -4988,232 +4988,232 @@
         <v>12</v>
       </c>
       <c r="GX5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="GY5" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="GZ5" t="n">
         <v>9</v>
       </c>
       <c r="HA5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="HB5" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="HC5" t="n">
+        <v>11</v>
+      </c>
+      <c r="HD5" t="n">
+        <v>17</v>
+      </c>
+      <c r="HE5" t="n">
+        <v>16</v>
+      </c>
+      <c r="HF5" t="n">
+        <v>16</v>
+      </c>
+      <c r="HG5" t="n">
+        <v>13</v>
+      </c>
+      <c r="HH5" t="n">
+        <v>18</v>
+      </c>
+      <c r="HI5" t="n">
+        <v>21</v>
+      </c>
+      <c r="HJ5" t="n">
+        <v>20</v>
+      </c>
+      <c r="HK5" t="n">
         <v>12</v>
       </c>
-      <c r="HD5" t="n">
+      <c r="HL5" t="n">
         <v>20</v>
       </c>
-      <c r="HE5" t="n">
-        <v>26</v>
-      </c>
-      <c r="HF5" t="n">
+      <c r="HM5" t="n">
         <v>24</v>
       </c>
-      <c r="HG5" t="n">
-        <v>24</v>
-      </c>
-      <c r="HH5" t="n">
-        <v>24</v>
-      </c>
-      <c r="HI5" t="n">
-        <v>18</v>
-      </c>
-      <c r="HJ5" t="n">
-        <v>13</v>
-      </c>
-      <c r="HK5" t="n">
-        <v>14</v>
-      </c>
-      <c r="HL5" t="n">
-        <v>15</v>
-      </c>
-      <c r="HM5" t="n">
-        <v>16</v>
-      </c>
       <c r="HN5" t="n">
+        <v>37</v>
+      </c>
+      <c r="HO5" t="n">
+        <v>37</v>
+      </c>
+      <c r="HP5" t="n">
         <v>39</v>
-      </c>
-      <c r="HO5" t="n">
-        <v>39</v>
-      </c>
-      <c r="HP5" t="n">
-        <v>40</v>
       </c>
       <c r="HQ5" t="n">
         <v>37</v>
       </c>
       <c r="HR5" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="HS5" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="HT5" t="n">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="HU5" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="HV5" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="HW5" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="HX5" t="n">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="HY5" t="n">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="HZ5" t="n">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="IA5" t="n">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="IB5" t="n">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="IC5" t="n">
         <v>74</v>
       </c>
       <c r="ID5" t="n">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="IE5" t="n">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="IF5" t="n">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="IG5" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="IH5" t="n">
         <v>8</v>
       </c>
       <c r="II5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="IJ5" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="IK5" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="IL5" t="n">
         <v>9</v>
       </c>
       <c r="IM5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="IN5" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="IO5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="IP5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="IQ5" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="IR5" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="IS5" t="n">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="IT5" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="IU5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="IV5" t="n">
         <v>15</v>
       </c>
       <c r="IW5" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="IX5" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="IY5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="IZ5" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="JA5" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="JB5" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="JC5" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="JD5" t="n">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="JE5" t="n">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="JF5" t="n">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="JG5" t="n">
+        <v>46</v>
+      </c>
+      <c r="JH5" t="n">
+        <v>37</v>
+      </c>
+      <c r="JI5" t="n">
+        <v>34</v>
+      </c>
+      <c r="JJ5" t="n">
         <v>41</v>
       </c>
-      <c r="JH5" t="n">
-        <v>30</v>
-      </c>
-      <c r="JI5" t="n">
-        <v>37</v>
-      </c>
-      <c r="JJ5" t="n">
-        <v>33</v>
-      </c>
       <c r="JK5" t="n">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="JL5" t="n">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="JM5" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="JN5" t="n">
+        <v>80</v>
+      </c>
+      <c r="JO5" t="n">
+        <v>86</v>
+      </c>
+      <c r="JP5" t="n">
+        <v>90</v>
+      </c>
+      <c r="JQ5" t="n">
+        <v>63</v>
+      </c>
+      <c r="JR5" t="n">
+        <v>76</v>
+      </c>
+      <c r="JS5" t="n">
+        <v>89</v>
+      </c>
+      <c r="JT5" t="n">
+        <v>93</v>
+      </c>
+      <c r="JU5" t="n">
         <v>70</v>
-      </c>
-      <c r="JO5" t="n">
-        <v>67</v>
-      </c>
-      <c r="JP5" t="n">
-        <v>83</v>
-      </c>
-      <c r="JQ5" t="n">
-        <v>79</v>
-      </c>
-      <c r="JR5" t="n">
-        <v>88</v>
-      </c>
-      <c r="JS5" t="n">
-        <v>82</v>
-      </c>
-      <c r="JT5" t="n">
-        <v>76</v>
-      </c>
-      <c r="JU5" t="n">
-        <v>76</v>
       </c>
     </row>
     <row r="6">
@@ -5253,217 +5253,217 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
+        <v>122</v>
+      </c>
+      <c r="O6" t="n">
+        <v>31</v>
+      </c>
+      <c r="P6" t="n">
+        <v>76</v>
+      </c>
+      <c r="Q6" t="n">
         <v>28</v>
       </c>
-      <c r="O6" t="n">
-        <v>3</v>
-      </c>
-      <c r="P6" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>2</v>
-      </c>
       <c r="R6" t="n">
-        <v>5</v>
+        <v>137</v>
       </c>
       <c r="S6" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U6" t="n">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="V6" t="n">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="W6" t="n">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="X6" t="n">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="Y6" t="n">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="Z6" t="n">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="AA6" t="n">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="AB6" t="n">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="AC6" t="n">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="AD6" t="n">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="AE6" t="n">
+        <v>12</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>57</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>67</v>
+      </c>
+      <c r="AH6" t="n">
         <v>42</v>
       </c>
-      <c r="AF6" t="n">
-        <v>35</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>31</v>
-      </c>
-      <c r="AH6" t="n">
+      <c r="AI6" t="n">
+        <v>98</v>
+      </c>
+      <c r="AJ6" t="n">
         <v>39</v>
       </c>
-      <c r="AI6" t="n">
-        <v>29</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>123</v>
-      </c>
       <c r="AK6" t="n">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="AL6" t="n">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="AM6" t="n">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="AN6" t="n">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="AO6" t="n">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="AP6" t="n">
-        <v>478</v>
+        <v>298</v>
       </c>
       <c r="AQ6" t="n">
-        <v>168</v>
+        <v>310</v>
       </c>
       <c r="AR6" t="n">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="AS6" t="n">
-        <v>339</v>
+        <v>120</v>
       </c>
       <c r="AT6" t="n">
-        <v>291</v>
+        <v>319</v>
       </c>
       <c r="AU6" t="n">
-        <v>416</v>
+        <v>158</v>
       </c>
       <c r="AV6" t="n">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="AW6" t="n">
-        <v>277</v>
+        <v>101</v>
       </c>
       <c r="AX6" t="n">
-        <v>171</v>
+        <v>327</v>
       </c>
       <c r="AY6" t="n">
-        <v>279</v>
+        <v>116</v>
       </c>
       <c r="AZ6" t="n">
-        <v>216</v>
+        <v>292</v>
       </c>
       <c r="BA6" t="n">
-        <v>237</v>
+        <v>397</v>
       </c>
       <c r="BB6" t="n">
-        <v>128</v>
+        <v>265</v>
       </c>
       <c r="BC6" t="n">
-        <v>401</v>
+        <v>281</v>
       </c>
       <c r="BD6" t="n">
-        <v>133</v>
+        <v>313</v>
       </c>
       <c r="BE6" t="n">
-        <v>263</v>
+        <v>221</v>
       </c>
       <c r="BF6" t="n">
-        <v>216</v>
+        <v>117</v>
       </c>
       <c r="BG6" t="n">
-        <v>398</v>
+        <v>213</v>
       </c>
       <c r="BH6" t="n">
-        <v>702</v>
+        <v>438</v>
       </c>
       <c r="BI6" t="n">
-        <v>93</v>
+        <v>212</v>
       </c>
       <c r="BJ6" t="n">
-        <v>1000</v>
+        <v>368</v>
       </c>
       <c r="BK6" t="n">
-        <v>785</v>
+        <v>317</v>
       </c>
       <c r="BL6" t="n">
-        <v>582</v>
+        <v>429</v>
       </c>
       <c r="BM6" t="n">
-        <v>287</v>
+        <v>329</v>
       </c>
       <c r="BN6" t="n">
-        <v>617</v>
+        <v>367</v>
       </c>
       <c r="BO6" t="n">
-        <v>171</v>
+        <v>520</v>
       </c>
       <c r="BP6" t="n">
-        <v>352</v>
+        <v>202</v>
       </c>
       <c r="BQ6" t="n">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="BR6" t="n">
-        <v>270</v>
+        <v>649</v>
       </c>
       <c r="BS6" t="n">
-        <v>397</v>
+        <v>322</v>
       </c>
       <c r="BT6" t="n">
-        <v>429</v>
+        <v>278</v>
       </c>
       <c r="BU6" t="n">
-        <v>367</v>
+        <v>297</v>
       </c>
       <c r="BV6" t="n">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="BW6" t="n">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="BX6" t="n">
-        <v>509</v>
+        <v>449</v>
       </c>
       <c r="BY6" t="n">
-        <v>335</v>
+        <v>762</v>
       </c>
       <c r="BZ6" t="n">
-        <v>648</v>
+        <v>686</v>
       </c>
       <c r="CA6" t="n">
-        <v>329</v>
+        <v>436</v>
       </c>
       <c r="CB6" t="n">
-        <v>889</v>
+        <v>487</v>
       </c>
       <c r="CC6" t="n">
-        <v>465</v>
+        <v>594</v>
       </c>
       <c r="CD6" t="n">
-        <v>784</v>
+        <v>1000</v>
       </c>
       <c r="CE6" t="n">
         <v>1000</v>
@@ -5472,10 +5472,10 @@
         <v>1000</v>
       </c>
       <c r="CG6" t="n">
-        <v>833</v>
+        <v>658</v>
       </c>
       <c r="CH6" t="n">
-        <v>1000</v>
+        <v>866</v>
       </c>
       <c r="CI6" t="n">
         <v>1000</v>
@@ -5484,7 +5484,7 @@
         <v>1000</v>
       </c>
       <c r="CK6" t="n">
-        <v>788</v>
+        <v>435</v>
       </c>
       <c r="CL6" t="n">
         <v>1000</v>
@@ -5502,13 +5502,13 @@
         <v>1000</v>
       </c>
       <c r="CQ6" t="n">
-        <v>674</v>
+        <v>1000</v>
       </c>
       <c r="CR6" t="n">
         <v>1000</v>
       </c>
       <c r="CS6" t="n">
-        <v>852</v>
+        <v>1000</v>
       </c>
       <c r="CT6" t="n">
         <v>1000</v>
@@ -5520,7 +5520,7 @@
         <v>1000</v>
       </c>
       <c r="CW6" t="n">
-        <v>1000</v>
+        <v>881</v>
       </c>
       <c r="CX6" t="n">
         <v>1000</v>

</xml_diff>